<commit_message>
move credentials to .env
move credentials to .env and retest the code
</commit_message>
<xml_diff>
--- a/Douban_books_result.xlsx
+++ b/Douban_books_result.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H490"/>
+  <dimension ref="A1:H491"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -712,12 +712,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>人生不设限</t>
+          <t>三国演义（全二册）</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Nick Vujicic / 彭蕙仙 / 天津社会科学院出版社 / 2011-6 / 29.80元</t>
+          <t>[明] 罗贯中 / 人民文学出版社 / 1998-05 / 39.50元</t>
         </is>
       </c>
       <c r="D9" s="2" t="n">
@@ -728,17 +728,13 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>基督教</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>我们有手有脚,有什么好抱怨的?</t>
-        </is>
-      </c>
+          <t>#人民文学 汉语文学 古典文学</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/6510070/</t>
+          <t>https://book.douban.com/subject/1019568/</t>
         </is>
       </c>
     </row>
@@ -748,12 +744,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>一生的远行</t>
+          <t>周国平人生哲思录</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>季羡林 / 华艺出版社 / 2008-6 / 42.00元</t>
+          <t>周国平 / 上海辞书出版社 / 2005-9 / 28.00元</t>
         </is>
       </c>
       <c r="D10" s="2" t="n">
@@ -764,17 +760,17 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>汉语文学 散文杂文</t>
+          <t>哲学 汉语文学 散文杂文</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>前面的留德十年还可以,后面的游记就大同小异了.</t>
+          <t>摘录式的文章,个人不太喜欢.</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/3115303/</t>
+          <t>https://book.douban.com/subject/1721111/</t>
         </is>
       </c>
     </row>
@@ -784,33 +780,29 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>小王子</t>
+          <t>善良丰富高贵</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>[法] 圣埃克絮佩里 / 周克希 / 上海译文出版社 / 2009-4 / 29.00元</t>
+          <t>周国平 / 万卷出版公司 / 2009-4 / 29.00元</t>
         </is>
       </c>
       <c r="D11" s="2" t="n">
         <v>41012</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>#上海译文 外国文学 法语文学</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>美丽的童话,结局有些感伤.总觉得作者的思想太过高深,隐藏在其中,难以完全体会.</t>
-        </is>
-      </c>
+          <t>汉语文学 散文杂文</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/3693974/</t>
+          <t>https://book.douban.com/subject/3673711/</t>
         </is>
       </c>
     </row>
@@ -820,29 +812,33 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>目送</t>
+          <t>妞妞</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>龙应台 / 生活·读书·新知三联书店 / 2009-10 / 39.00元</t>
+          <t>周国平 / 人民文学出版社 / 2009-4 / 20.00元</t>
         </is>
       </c>
       <c r="D12" s="2" t="n">
         <v>41012</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>散文杂文</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr"/>
+          <t>汉语文学 散文杂文</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>我觉得是周国平写得最好的一本书.</t>
+        </is>
+      </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/3995526/</t>
+          <t>https://book.douban.com/subject/3669595/</t>
         </is>
       </c>
     </row>
@@ -852,29 +848,33 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>名人传</t>
+          <t>欧·亨利短篇小说选</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>(法)罗曼·罗兰 / 张冠尧、艾珉 / 人民文学出版社 / 1991 / 18.00元</t>
+          <t>欧·亨利 / 王永年 / 人民文学出版社 / 2003-1 / 16.00元</t>
         </is>
       </c>
       <c r="D13" s="2" t="n">
         <v>41012</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>#人民文学 传记 外国文学 法语文学</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr"/>
+          <t>#人民文学 英语文学 外国文学</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>小人物的故事，他独具特色的结尾。</t>
+        </is>
+      </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/3181294/</t>
+          <t>https://book.douban.com/subject/3200734/</t>
         </is>
       </c>
     </row>
@@ -884,33 +884,29 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>妞妞</t>
+          <t>目送</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>周国平 / 人民文学出版社 / 2009-4 / 20.00元</t>
+          <t>龙应台 / 生活·读书·新知三联书店 / 2009-10 / 39.00元</t>
         </is>
       </c>
       <c r="D14" s="2" t="n">
         <v>41012</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>汉语文学 散文杂文</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>我觉得是周国平写得最好的一本书.</t>
-        </is>
-      </c>
+          <t>散文杂文</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/3669595/</t>
+          <t>https://book.douban.com/subject/3995526/</t>
         </is>
       </c>
     </row>
@@ -920,29 +916,33 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>善良丰富高贵</t>
+          <t>小王子</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>周国平 / 万卷出版公司 / 2009-4 / 29.00元</t>
+          <t>[法] 圣埃克絮佩里 / 周克希 / 上海译文出版社 / 2009-4 / 29.00元</t>
         </is>
       </c>
       <c r="D15" s="2" t="n">
         <v>41012</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>汉语文学 散文杂文</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr"/>
+          <t>#上海译文 外国文学 法语文学</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>美丽的童话,结局有些感伤.总觉得作者的思想太过高深,隐藏在其中,难以完全体会.</t>
+        </is>
+      </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/3673711/</t>
+          <t>https://book.douban.com/subject/3693974/</t>
         </is>
       </c>
     </row>
@@ -952,12 +952,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>周国平人生哲思录</t>
+          <t>一生的远行</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>周国平 / 上海辞书出版社 / 2005-9 / 28.00元</t>
+          <t>季羡林 / 华艺出版社 / 2008-6 / 42.00元</t>
         </is>
       </c>
       <c r="D16" s="2" t="n">
@@ -968,17 +968,17 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>哲学 汉语文学 散文杂文</t>
+          <t>汉语文学 散文杂文</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>摘录式的文章,个人不太喜欢.</t>
+          <t>前面的留德十年还可以,后面的游记就大同小异了.</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/1721111/</t>
+          <t>https://book.douban.com/subject/3115303/</t>
         </is>
       </c>
     </row>
@@ -988,29 +988,29 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>三国演义（全二册）</t>
+          <t>名人传</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>[明] 罗贯中 / 人民文学出版社 / 1998-05 / 39.50元</t>
+          <t>(法)罗曼·罗兰 / 张冠尧、艾珉 / 人民文学出版社 / 1991 / 18.00元</t>
         </is>
       </c>
       <c r="D17" s="2" t="n">
         <v>41012</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>#人民文学 汉语文学 古典文学</t>
+          <t>#人民文学 传记 外国文学 法语文学</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/1019568/</t>
+          <t>https://book.douban.com/subject/3181294/</t>
         </is>
       </c>
     </row>
@@ -1020,12 +1020,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>欧·亨利短篇小说选</t>
+          <t>人生不设限</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>欧·亨利 / 王永年 / 人民文学出版社 / 2003-1 / 16.00元</t>
+          <t>Nick Vujicic / 彭蕙仙 / 天津社会科学院出版社 / 2011-6 / 29.80元</t>
         </is>
       </c>
       <c r="D18" s="2" t="n">
@@ -1036,17 +1036,17 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>#人民文学 英语文学 外国文学</t>
+          <t>基督教</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>小人物的故事，他独具特色的结尾。</t>
+          <t>我们有手有脚,有什么好抱怨的?</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/3200734/</t>
+          <t>https://book.douban.com/subject/6510070/</t>
         </is>
       </c>
     </row>
@@ -1188,29 +1188,29 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>我们都爱普鲁斯特</t>
+          <t>英伦风格小屋</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>[美] 安德烈·艾西蒙 / 河西 / 上海三联书店 / 2010-10 / 28.00元</t>
+          <t>[日] 井行庆子 / 宋佳静 / 中信出版社 / 2010年11月 / 35.00元</t>
         </is>
       </c>
       <c r="D23" s="2" t="n">
         <v>41230</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>#三联书店 普鲁斯特 外国文学 文学评论 法语文学</t>
+          <t>应用书籍</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/5336382/</t>
+          <t>https://book.douban.com/subject/5363512/</t>
         </is>
       </c>
     </row>
@@ -1220,12 +1220,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>英伦风格小屋</t>
+          <t>爱默生集</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>[日] 井行庆子 / 宋佳静 / 中信出版社 / 2010年11月 / 35.00元</t>
+          <t>范圣宇、[美] 拉尔夫·瓦尔多·爱默生 / 花城出版社 / 2008-1 / 45.00元</t>
         </is>
       </c>
       <c r="D24" s="2" t="n">
@@ -1236,13 +1236,17 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>应用书籍</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr"/>
+          <t>外国文学 英语文学</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>翻译得有些生涩，篇幅很长，要耐心看。</t>
+        </is>
+      </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/5363512/</t>
+          <t>https://book.douban.com/subject/2984505/</t>
         </is>
       </c>
     </row>
@@ -1252,33 +1256,29 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>爱默生集</t>
+          <t>我们都爱普鲁斯特</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>范圣宇、[美] 拉尔夫·瓦尔多·爱默生 / 花城出版社 / 2008-1 / 45.00元</t>
+          <t>[美] 安德烈·艾西蒙 / 河西 / 上海三联书店 / 2010-10 / 28.00元</t>
         </is>
       </c>
       <c r="D25" s="2" t="n">
         <v>41230</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>外国文学 英语文学</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>翻译得有些生涩，篇幅很长，要耐心看。</t>
-        </is>
-      </c>
+          <t>#三联书店 普鲁斯特 外国文学 文学评论 法语文学</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/2984505/</t>
+          <t>https://book.douban.com/subject/5336382/</t>
         </is>
       </c>
     </row>
@@ -1496,33 +1496,29 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>1973年的弹子球</t>
+          <t>福尔摩斯探案精选</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>(日)村上春树 / 林少华 / 上海译文出版社 / 2008-8 / 15.00元</t>
+          <t>柯南·道尔 / 梅绍武、屠珍 / 上海译文出版社 / 2010-8 / 35.00元</t>
         </is>
       </c>
       <c r="D32" s="2" t="n">
         <v>41463</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>日语文学 外国文学 #上海译文</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>我完全看不懂</t>
-        </is>
-      </c>
+          <t>#上海译文 英语文学 侦探小说 外国文学</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/3168460/</t>
+          <t>https://book.douban.com/subject/5041577/</t>
         </is>
       </c>
     </row>
@@ -1532,29 +1528,33 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>福尔摩斯探案精选</t>
+          <t>1973年的弹子球</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>柯南·道尔 / 梅绍武、屠珍 / 上海译文出版社 / 2010-8 / 35.00元</t>
+          <t>(日)村上春树 / 林少华 / 上海译文出版社 / 2008-8 / 15.00元</t>
         </is>
       </c>
       <c r="D33" s="2" t="n">
         <v>41463</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>#上海译文 英语文学 侦探小说 外国文学</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr"/>
+          <t>日语文学 外国文学 #上海译文</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>我完全看不懂</t>
+        </is>
+      </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/5041577/</t>
+          <t>https://book.douban.com/subject/3168460/</t>
         </is>
       </c>
     </row>
@@ -2544,29 +2544,33 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>侠盗亚森·罗平</t>
+          <t>身份的焦虑</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>[法] 勒布朗 / 周克希 / 华东师范大学出版社 / 2012-1 / 20.00元</t>
+          <t>[英] 阿兰·德波顿 / 陈广兴、南治国 / 上海译文出版社 / 2009-4 / 27.00</t>
         </is>
       </c>
       <c r="D62" s="2" t="n">
         <v>41742</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>#周克希译文集 外国文学 法语文学</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr"/>
+          <t>英语文学 #上海译文</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>不知为何，竟然没有读下去。我觉得阿兰的书，还是小说更好一些。身份的焦虑，说到底，唯一的解决办法，都是对价值的重估。</t>
+        </is>
+      </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/6893859/</t>
+          <t>https://book.douban.com/subject/3669408/</t>
         </is>
       </c>
     </row>
@@ -2576,33 +2580,29 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>身份的焦虑</t>
+          <t>唐宋词选</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>[英] 阿兰·德波顿 / 陈广兴、南治国 / 上海译文出版社 / 2009-4 / 27.00</t>
+          <t>夏承焘 盛韬青 选注 / 中国青年出版社 / 1959-11 / 0.64元</t>
         </is>
       </c>
       <c r="D63" s="2" t="n">
         <v>41742</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>英语文学 #上海译文</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>不知为何，竟然没有读下去。我觉得阿兰的书，还是小说更好一些。身份的焦虑，说到底，唯一的解决办法，都是对价值的重估。</t>
-        </is>
-      </c>
+          <t>汉语文学 古典文学</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/3669408/</t>
+          <t>https://book.douban.com/subject/2027159/</t>
         </is>
       </c>
     </row>
@@ -2612,12 +2612,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>唐宋词选</t>
+          <t>侠盗亚森·罗平</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>夏承焘 盛韬青 选注 / 中国青年出版社 / 1959-11 / 0.64元</t>
+          <t>[法] 勒布朗 / 周克希 / 华东师范大学出版社 / 2012-1 / 20.00元</t>
         </is>
       </c>
       <c r="D64" s="2" t="n">
@@ -2628,13 +2628,13 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>汉语文学 古典文学</t>
+          <t>#周克希译文集 外国文学 法语文学</t>
         </is>
       </c>
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/2027159/</t>
+          <t>https://book.douban.com/subject/6893859/</t>
         </is>
       </c>
     </row>
@@ -2752,12 +2752,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>世界别为我担心</t>
+          <t>蓝石头</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>幾米 / 海豚出版社 / 2012-1-1 / 28.00元</t>
+          <t>幾米 / 现代出版社 / 2006-4 / 36.00元</t>
         </is>
       </c>
       <c r="D68" s="2" t="n">
@@ -2774,7 +2774,7 @@
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/6889910/</t>
+          <t>https://book.douban.com/subject/1761056/</t>
         </is>
       </c>
     </row>
@@ -2784,12 +2784,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>蓝石头</t>
+          <t>世界别为我担心</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>幾米 / 现代出版社 / 2006-4 / 36.00元</t>
+          <t>幾米 / 海豚出版社 / 2012-1-1 / 28.00元</t>
         </is>
       </c>
       <c r="D69" s="2" t="n">
@@ -2806,7 +2806,7 @@
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/1761056/</t>
+          <t>https://book.douban.com/subject/6889910/</t>
         </is>
       </c>
     </row>
@@ -2816,33 +2816,33 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>我不是来演讲的</t>
+          <t>红楼梦</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>[哥伦比亚] 加西亚·马尔克斯 / 李静 / 南海出版公司 / 2012-1 / 28.00元</t>
+          <t>[清] 曹雪芹 著、高鹗 / 人民文学出版社 / 1996-12 / 59.70元</t>
         </is>
       </c>
       <c r="D70" s="2" t="n">
         <v>41761</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>西语文学 外国文学 #新经典</t>
+          <t>#人民文学 汉语文学 古典文学</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>P7：对我而言，文学创作就和登台演讲一样，都是被逼的。P24:我斗胆认为，是拉丁美洲异乎寻常的现实，而不仅仅是其文学表现形式，引起了瑞典文学院的极大关注。P37：科学只与科学家有关的想法本身是反科学的，正如诗歌只与诗人有关的想法反诗歌。P38：更糟的是，在这一百年里，我们还丧失了十九世纪最可贵的美德：狂热的理想主义和对感情的重视，对爱的恐惧。P94:广播剧之父费力克斯·B·B卡格内特说：“人爱流眼泪，而我给他们流眼泪的借口，仅此而已。”P137:一百万人决定去读一本全凭一人独坐陋室，用二十八个字母，两根指头敲出来的书，想想都觉得疯狂。</t>
+          <t>缘起之诗“满纸荒唐言，一把辛酸泪。都云作者痴，谁解其中味。”到结语“说到新酸处，荒唐愈可悲。由来同一梦，休笑世人痴。”曹雪芹先生批阅十载，增删五次，终于完成此书。要想字字读来皆是血，必须要十年辛苦不寻常啊！</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/6890669/</t>
+          <t>https://book.douban.com/subject/1007305/</t>
         </is>
       </c>
     </row>
@@ -2852,33 +2852,33 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>红楼梦</t>
+          <t>我不是来演讲的</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>[清] 曹雪芹 著、高鹗 / 人民文学出版社 / 1996-12 / 59.70元</t>
+          <t>[哥伦比亚] 加西亚·马尔克斯 / 李静 / 南海出版公司 / 2012-1 / 28.00元</t>
         </is>
       </c>
       <c r="D71" s="2" t="n">
         <v>41761</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>#人民文学 汉语文学 古典文学</t>
+          <t>西语文学 外国文学 #新经典</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>缘起之诗“满纸荒唐言，一把辛酸泪。都云作者痴，谁解其中味。”到结语“说到新酸处，荒唐愈可悲。由来同一梦，休笑世人痴。”曹雪芹先生批阅十载，增删五次，终于完成此书。要想字字读来皆是血，必须要十年辛苦不寻常啊！</t>
+          <t>P7：对我而言，文学创作就和登台演讲一样，都是被逼的。P24:我斗胆认为，是拉丁美洲异乎寻常的现实，而不仅仅是其文学表现形式，引起了瑞典文学院的极大关注。P37：科学只与科学家有关的想法本身是反科学的，正如诗歌只与诗人有关的想法反诗歌。P38：更糟的是，在这一百年里，我们还丧失了十九世纪最可贵的美德：狂热的理想主义和对感情的重视，对爱的恐惧。P94:广播剧之父费力克斯·B·B卡格内特说：“人爱流眼泪，而我给他们流眼泪的借口，仅此而已。”P137:一百万人决定去读一本全凭一人独坐陋室，用二十八个字母，两根指头敲出来的书，想想都觉得疯狂。</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/1007305/</t>
+          <t>https://book.douban.com/subject/6890669/</t>
         </is>
       </c>
     </row>
@@ -3024,12 +3024,12 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>活着</t>
+          <t>三剑客</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>余华 / 作家出版社 / 2012-8 / 28.00元</t>
+          <t>[法]大仲马 / 周克希 / 华东师范大学出版社 / 2012-6 / 68.00元</t>
         </is>
       </c>
       <c r="D76" s="2" t="n">
@@ -3040,17 +3040,17 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>汉语文学 现当代文学</t>
+          <t>#周克希译文集 外国文学 法语文学</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>断断续续地读完了。倒不是不能快起来，而是故事本身实在压抑沉闷。作者的叙述方式非常冷峻，故事又很悲情。这种对比表现出了当时中国近乎荒谬的现实。</t>
+          <t>我看到最后只想知道：凯蒂的结局是什么？</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/4913064/</t>
+          <t>https://book.douban.com/subject/10559575/</t>
         </is>
       </c>
     </row>
@@ -3060,12 +3060,12 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>三剑客</t>
+          <t>活着</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>[法]大仲马 / 周克希 / 华东师范大学出版社 / 2012-6 / 68.00元</t>
+          <t>余华 / 作家出版社 / 2012-8 / 28.00元</t>
         </is>
       </c>
       <c r="D77" s="2" t="n">
@@ -3076,17 +3076,17 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>#周克希译文集 外国文学 法语文学</t>
+          <t>汉语文学 现当代文学</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>我看到最后只想知道：凯蒂的结局是什么？</t>
+          <t>断断续续地读完了。倒不是不能快起来，而是故事本身实在压抑沉闷。作者的叙述方式非常冷峻，故事又很悲情。这种对比表现出了当时中国近乎荒谬的现实。</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/10559575/</t>
+          <t>https://book.douban.com/subject/4913064/</t>
         </is>
       </c>
     </row>
@@ -3564,33 +3564,33 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>The Time Machine</t>
+          <t>The Structure of Scientific Revolutions</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>H. G. Wells / Dover Publications / 1995-4-3 / USD 2.00</t>
+          <t>Thomas S. Kuhn / University Of Chicago Press / 2012-4-30 / USD 15.00</t>
         </is>
       </c>
       <c r="D91" s="2" t="n">
         <v>41983</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>原版 外国文学 英语文学</t>
+          <t>自然科学 原版</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>GPC Requirement. Finished the first two three chapters.</t>
+          <t>P12:These transformations of the paradigms of physical optics are scientific revolutions, and the successive transition from one paradigm to another via revolution is the usual developmental pattern of mature science. P169: changes of paradigm carry scientists and those who learn from them closer and closer to the truth.</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/3611809/</t>
+          <t>https://book.douban.com/subject/7015878/</t>
         </is>
       </c>
     </row>
@@ -3636,33 +3636,33 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>The Structure of Scientific Revolutions</t>
+          <t>The Time Machine</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Thomas S. Kuhn / University Of Chicago Press / 2012-4-30 / USD 15.00</t>
+          <t>H. G. Wells / Dover Publications / 1995-4-3 / USD 2.00</t>
         </is>
       </c>
       <c r="D93" s="2" t="n">
         <v>41983</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>自然科学 原版</t>
+          <t>原版 外国文学 英语文学</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>P12:These transformations of the paradigms of physical optics are scientific revolutions, and the successive transition from one paradigm to another via revolution is the usual developmental pattern of mature science. P169: changes of paradigm carry scientists and those who learn from them closer and closer to the truth.</t>
+          <t>GPC Requirement. Finished the first two three chapters.</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/7015878/</t>
+          <t>https://book.douban.com/subject/3611809/</t>
         </is>
       </c>
     </row>
@@ -6272,12 +6272,12 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>哈利·波特与火焰杯</t>
+          <t>哈利·波特与阿兹卡班的囚徒</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>[英] J. K. 罗琳 / 马爱新 / 人民文学出版社 / 2001-5 / 39.80元</t>
+          <t>[英] J. K. 罗琳 / 郑须弥 / 人民文学出版社 / 2000-9 / 26.50元</t>
         </is>
       </c>
       <c r="D167" s="2" t="n">
@@ -6294,7 +6294,7 @@
       <c r="G167" t="inlineStr"/>
       <c r="H167" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/1009257/</t>
+          <t>https://book.douban.com/subject/1071241/</t>
         </is>
       </c>
     </row>
@@ -6304,19 +6304,19 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>哈利·波特与阿兹卡班的囚徒</t>
+          <t>哈利·波特与密室</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>[英] J. K. 罗琳 / 郑须弥 / 人民文学出版社 / 2000-9 / 26.50元</t>
+          <t>[英] J. K. 罗琳 / 马爱新 / 人民文学出版社 / 2000-9 / 22.00元</t>
         </is>
       </c>
       <c r="D168" s="2" t="n">
         <v>42569</v>
       </c>
       <c r="E168" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F168" t="inlineStr">
         <is>
@@ -6326,7 +6326,7 @@
       <c r="G168" t="inlineStr"/>
       <c r="H168" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/1071241/</t>
+          <t>https://book.douban.com/subject/1039487/</t>
         </is>
       </c>
     </row>
@@ -6336,12 +6336,12 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>哈利·波特与死亡圣器</t>
+          <t>哈利·波特与火焰杯</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>[英] J. K. 罗琳 / 马爱农、马爱新 / 人民文学出版社 / 2007-10 / 66.00元</t>
+          <t>[英] J. K. 罗琳 / 马爱新 / 人民文学出版社 / 2001-5 / 39.80元</t>
         </is>
       </c>
       <c r="D169" s="2" t="n">
@@ -6358,7 +6358,7 @@
       <c r="G169" t="inlineStr"/>
       <c r="H169" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/2295163/</t>
+          <t>https://book.douban.com/subject/1009257/</t>
         </is>
       </c>
     </row>
@@ -6432,19 +6432,19 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>哈利·波特与密室</t>
+          <t>哈利·波特与死亡圣器</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>[英] J. K. 罗琳 / 马爱新 / 人民文学出版社 / 2000-9 / 22.00元</t>
+          <t>[英] J. K. 罗琳 / 马爱农、马爱新 / 人民文学出版社 / 2007-10 / 66.00元</t>
         </is>
       </c>
       <c r="D172" s="2" t="n">
         <v>42569</v>
       </c>
       <c r="E172" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F172" t="inlineStr">
         <is>
@@ -6454,7 +6454,7 @@
       <c r="G172" t="inlineStr"/>
       <c r="H172" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/1039487/</t>
+          <t>https://book.douban.com/subject/2295163/</t>
         </is>
       </c>
     </row>
@@ -7400,33 +7400,33 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>The Elements of Style</t>
+          <t>呼啸山庄</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>William Strunk Jr. / Dover Publications / 2006-5-26 / USD 3.95</t>
+          <t>[英] 艾米莉·勃朗特 / 方平 / 上海译文出版社 / 2010-8-1 / 23.00元</t>
         </is>
       </c>
       <c r="D199" s="2" t="n">
         <v>42912</v>
       </c>
       <c r="E199" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F199" t="inlineStr">
         <is>
-          <t>原版 外国文学 英语文学 文学评论</t>
+          <t>英语文学 外国文学 #上海译文</t>
         </is>
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>short but impressive</t>
+          <t>我几乎没读过主人公（希克利）是这么讨人厌的小说了，几乎所有其他角色都不喜欢他。有时我甚至觉得故事毫无意义：一个虐待狂复仇的故事，简直可以改名为《呼啸山庄复仇记》。不过最后四章还是升华了整个主题的。方平老师的译文流畅，不过我更喜欢的是他所写的序，很有启发性，推荐读完书后再读。</t>
         </is>
       </c>
       <c r="H199" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/1824592/</t>
+          <t>https://book.douban.com/subject/5273041/</t>
         </is>
       </c>
     </row>
@@ -7436,33 +7436,33 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>呼啸山庄</t>
+          <t>The Elements of Style</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>[英] 艾米莉·勃朗特 / 方平 / 上海译文出版社 / 2010-8-1 / 23.00元</t>
+          <t>William Strunk Jr. / Dover Publications / 2006-5-26 / USD 3.95</t>
         </is>
       </c>
       <c r="D200" s="2" t="n">
         <v>42912</v>
       </c>
       <c r="E200" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F200" t="inlineStr">
         <is>
-          <t>英语文学 外国文学 #上海译文</t>
+          <t>原版 外国文学 英语文学 文学评论</t>
         </is>
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>我几乎没读过主人公（希克利）是这么讨人厌的小说了，几乎所有其他角色都不喜欢他。有时我甚至觉得故事毫无意义：一个虐待狂复仇的故事，简直可以改名为《呼啸山庄复仇记》。不过最后四章还是升华了整个主题的。方平老师的译文流畅，不过我更喜欢的是他所写的序，很有启发性，推荐读完书后再读。</t>
+          <t>short but impressive</t>
         </is>
       </c>
       <c r="H200" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/5273041/</t>
+          <t>https://book.douban.com/subject/1824592/</t>
         </is>
       </c>
     </row>
@@ -8120,12 +8120,12 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>大家都有病</t>
+          <t>我的职业是小说家</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>朱德庸 / 现代出版社 / 2011-5 / 36.00元</t>
+          <t>[日] 村上春树 / 施小炜 / 南海出版公司 / 2017-1 / 45.00元</t>
         </is>
       </c>
       <c r="D219" s="2" t="n">
@@ -8136,17 +8136,17 @@
       </c>
       <c r="F219" t="inlineStr">
         <is>
-          <t>绘本</t>
+          <t>日语文学 外国文学 #新经典</t>
         </is>
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>我也有病，鉴定完毕</t>
+          <t>好友所赠。感觉村上是个温暖的大叔，会和你在午后泡杯咖啡好好聊天，虽然有时候废话有些多。这本书叫做《我的职业是小说家》，但是实际上内容（正如他自己在后记中所说）讲的是：我也不知道自己是怎么成为小说家的。不过这样也好，感觉村上其实并不是一个日本本土化的小说家，倒是和欧美的一些作家比较接近。这样一来，他的气质和我所构想的以自杀著称的日本小说家倒是不太一样。不过其实这么想，也是进入了一个stereotype，作家干嘛非要是那种和其他人不一样的人呢？就像村上自己说的，小说家干嘛非要是艺术家呢？小说家一边创作小说一边被小说所创作着，反正都是有缺陷的人写的有缺陷的小说，那只要写出好东西，过程读者就不必要深究了嘛。</t>
         </is>
       </c>
       <c r="H219" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/6114393/</t>
+          <t>https://book.douban.com/subject/26889236/</t>
         </is>
       </c>
     </row>
@@ -8156,12 +8156,12 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>我的职业是小说家</t>
+          <t>大家都有病</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>[日] 村上春树 / 施小炜 / 南海出版公司 / 2017-1 / 45.00元</t>
+          <t>朱德庸 / 现代出版社 / 2011-5 / 36.00元</t>
         </is>
       </c>
       <c r="D220" s="2" t="n">
@@ -8172,17 +8172,17 @@
       </c>
       <c r="F220" t="inlineStr">
         <is>
-          <t>日语文学 外国文学 #新经典</t>
+          <t>绘本</t>
         </is>
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>好友所赠。感觉村上是个温暖的大叔，会和你在午后泡杯咖啡好好聊天，虽然有时候废话有些多。这本书叫做《我的职业是小说家》，但是实际上内容（正如他自己在后记中所说）讲的是：我也不知道自己是怎么成为小说家的。不过这样也好，感觉村上其实并不是一个日本本土化的小说家，倒是和欧美的一些作家比较接近。这样一来，他的气质和我所构想的以自杀著称的日本小说家倒是不太一样。不过其实这么想，也是进入了一个stereotype，作家干嘛非要是那种和其他人不一样的人呢？就像村上自己说的，小说家干嘛非要是艺术家呢？小说家一边创作小说一边被小说所创作着，反正都是有缺陷的人写的有缺陷的小说，那只要写出好东西，过程读者就不必要深究了嘛。</t>
+          <t>我也有病，鉴定完毕</t>
         </is>
       </c>
       <c r="H220" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/26889236/</t>
+          <t>https://book.douban.com/subject/6114393/</t>
         </is>
       </c>
     </row>
@@ -8516,12 +8516,12 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>让数字说话</t>
+          <t>昨日之旅</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>孙含晖(金十七)、王苏颖、阎歌 / 机械工业出版社 / 2016-3-4 / 45.00元</t>
+          <t>[奥] 斯特凡•茨威格 / 关惠文 / 上海译文出版社 / 2016-10 / 36</t>
         </is>
       </c>
       <c r="D230" s="2" t="n">
@@ -8532,17 +8532,17 @@
       </c>
       <c r="F230" t="inlineStr">
         <is>
-          <t>应用书籍 审计</t>
+          <t>#上海译文 外国文学 德语文学</t>
         </is>
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>感谢Jiamin，虽然没读完，但是也见证了我两年的审计工作。</t>
+          <t xml:space="preserve">2019第四本茨威格。《情感的迷惘》：无法理解与被理解的爱。《孪生姐妹》：在所有浮华全都过去后，只有谦卑才是永恒的真理。《奇妙之夜》：行尸走肉意外之下终于发现了让自己心潮澎湃的秘密。《一颗心的沦亡》：再一次证明了，一个人太多愁善感，是很累的。《旧书商门德尔》：不管在任何时候，哪怕在战争时期，一个人都可以活在自己的精神世界中。《巧识新艺》：如何细致入微地观察一个小偷。《昨日之旅》：过去的，终究不会再来。《是他吗》：升米恩斗米仇，对动物也是如此。到此为止，上译这个系列的所有小说我都读完了，总结下来茨威格：1.以细腻的心理描写见长 2. 以普通人的短暂但汹涌的感情为主线 3. 写法上喜欢借旁观者写（有点像《十日谈》？）。 </t>
         </is>
       </c>
       <c r="H230" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/26746460/</t>
+          <t>https://book.douban.com/subject/26828751/</t>
         </is>
       </c>
     </row>
@@ -8552,33 +8552,33 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>四大那些事</t>
+          <t>让数字说话</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>啃哥张驰 / 中国市场出版社 / 2015-1-1 / 39.00</t>
+          <t>孙含晖(金十七)、王苏颖、阎歌 / 机械工业出版社 / 2016-3-4 / 45.00元</t>
         </is>
       </c>
       <c r="D231" s="2" t="n">
         <v>43579</v>
       </c>
       <c r="E231" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F231" t="inlineStr">
         <is>
-          <t>审计 应用书籍</t>
+          <t>应用书籍 审计</t>
         </is>
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>和《让数字说话》一样，也是Jiamin所赠。感谢她。前面的八卦还是很有意思的。</t>
+          <t>感谢Jiamin，虽然没读完，但是也见证了我两年的审计工作。</t>
         </is>
       </c>
       <c r="H231" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/26318428/</t>
+          <t>https://book.douban.com/subject/26746460/</t>
         </is>
       </c>
     </row>
@@ -8588,33 +8588,33 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>昨日之旅</t>
+          <t>四大那些事</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>[奥] 斯特凡•茨威格 / 关惠文 / 上海译文出版社 / 2016-10 / 36</t>
+          <t>啃哥张驰 / 中国市场出版社 / 2015-1-1 / 39.00</t>
         </is>
       </c>
       <c r="D232" s="2" t="n">
         <v>43579</v>
       </c>
       <c r="E232" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F232" t="inlineStr">
         <is>
-          <t>#上海译文 外国文学 德语文学</t>
+          <t>审计 应用书籍</t>
         </is>
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t xml:space="preserve">2019第四本茨威格。《情感的迷惘》：无法理解与被理解的爱。《孪生姐妹》：在所有浮华全都过去后，只有谦卑才是永恒的真理。《奇妙之夜》：行尸走肉意外之下终于发现了让自己心潮澎湃的秘密。《一颗心的沦亡》：再一次证明了，一个人太多愁善感，是很累的。《旧书商门德尔》：不管在任何时候，哪怕在战争时期，一个人都可以活在自己的精神世界中。《巧识新艺》：如何细致入微地观察一个小偷。《昨日之旅》：过去的，终究不会再来。《是他吗》：升米恩斗米仇，对动物也是如此。到此为止，上译这个系列的所有小说我都读完了，总结下来茨威格：1.以细腻的心理描写见长 2. 以普通人的短暂但汹涌的感情为主线 3. 写法上喜欢借旁观者写（有点像《十日谈》？）。 </t>
+          <t>和《让数字说话》一样，也是Jiamin所赠。感谢她。前面的八卦还是很有意思的。</t>
         </is>
       </c>
       <c r="H232" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/26828751/</t>
+          <t>https://book.douban.com/subject/26318428/</t>
         </is>
       </c>
     </row>
@@ -8940,19 +8940,19 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>芬兰人的噩梦</t>
+          <t>我可以咬一口吗</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>[芬]卡罗利娜·科尔霍宁 / 李浚帆 / 广西师范大学出版社 / 2018-6 / 39.00</t>
+          <t>[美] 莉兹·克里莫 / 周高逸 / 天津人民出版社 / 2016-4 / 39.00元</t>
         </is>
       </c>
       <c r="D242" s="2" t="n">
         <v>43654</v>
       </c>
       <c r="E242" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F242" t="inlineStr">
         <is>
@@ -8961,12 +8961,12 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>虽然页数有点少，但是从中也可以看出芬兰人和广大网民有些类似......</t>
+          <t>好可爱！</t>
         </is>
       </c>
       <c r="H242" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/30234130/</t>
+          <t>https://book.douban.com/subject/26755503/</t>
         </is>
       </c>
     </row>
@@ -8976,12 +8976,12 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>我可以咬一口吗</t>
+          <t>你今天真好看</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>[美] 莉兹·克里莫 / 周高逸 / 天津人民出版社 / 2016-4 / 39.00元</t>
+          <t>[美]莉兹•克里莫 / 周高逸 / 天津人民出版社 / 2015-8 / 39.00元</t>
         </is>
       </c>
       <c r="D243" s="2" t="n">
@@ -8997,12 +8997,12 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>好可爱！</t>
+          <t>在家养病，想读点轻松的东西。真可爱！</t>
         </is>
       </c>
       <c r="H243" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/26755503/</t>
+          <t>https://book.douban.com/subject/26602392/</t>
         </is>
       </c>
     </row>
@@ -9012,19 +9012,19 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>你今天真好看</t>
+          <t>芬兰人的噩梦</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>[美]莉兹•克里莫 / 周高逸 / 天津人民出版社 / 2015-8 / 39.00元</t>
+          <t>[芬]卡罗利娜·科尔霍宁 / 李浚帆 / 广西师范大学出版社 / 2018-6 / 39.00</t>
         </is>
       </c>
       <c r="D244" s="2" t="n">
         <v>43654</v>
       </c>
       <c r="E244" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F244" t="inlineStr">
         <is>
@@ -9033,12 +9033,12 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>在家养病，想读点轻松的东西。真可爱！</t>
+          <t>虽然页数有点少，但是从中也可以看出芬兰人和广大网民有些类似......</t>
         </is>
       </c>
       <c r="H244" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/26602392/</t>
+          <t>https://book.douban.com/subject/30234130/</t>
         </is>
       </c>
     </row>
@@ -9192,12 +9192,12 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>ONE-PUNCH MAN 一拳超人 06</t>
+          <t>ONE-PUNCH MAN 一拳超人 19</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2015-12-2 / NT$100</t>
+          <t>ONE、村田雄介 / 吳勵誠 / 東立 / 2019-6-17 / NT$100</t>
         </is>
       </c>
       <c r="D249" s="2" t="n">
@@ -9214,7 +9214,7 @@
       <c r="G249" t="inlineStr"/>
       <c r="H249" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/26429149/</t>
+          <t>https://book.douban.com/subject/34434070/</t>
         </is>
       </c>
     </row>
@@ -9224,12 +9224,12 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>ONE-PUNCH MAN 一拳超人 08</t>
+          <t>ONE PUNCH MAN一拳超人 18</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2016-1-29 / NT$100</t>
+          <t>村田雄介、ONE / 吳勵誠 / 東立出版社 / 2019-2-20 / NT100</t>
         </is>
       </c>
       <c r="D250" s="2" t="n">
@@ -9246,7 +9246,7 @@
       <c r="G250" t="inlineStr"/>
       <c r="H250" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/26429151/</t>
+          <t>https://book.douban.com/subject/30380122/</t>
         </is>
       </c>
     </row>
@@ -9256,12 +9256,12 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>ONE-PUNCH MAN 一拳超人 09</t>
+          <t>ONE PUNCH MAN一拳超人 17</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2016-2-4 / NT$100</t>
+          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2018-11-15 / NT100</t>
         </is>
       </c>
       <c r="D251" s="2" t="n">
@@ -9278,7 +9278,7 @@
       <c r="G251" t="inlineStr"/>
       <c r="H251" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/26577748/</t>
+          <t>https://book.douban.com/subject/30278079/</t>
         </is>
       </c>
     </row>
@@ -9288,12 +9288,12 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>ONE-PUNCH MAN 一拳超人 07</t>
+          <t>ONE-PUNCH MAN 一拳超人 16</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2015-12-21 / NT$100</t>
+          <t>ONE、村田雄介 / 吳勵誠 / 東立 / 2018-5-30 / NT$100</t>
         </is>
       </c>
       <c r="D252" s="2" t="n">
@@ -9310,7 +9310,7 @@
       <c r="G252" t="inlineStr"/>
       <c r="H252" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/26429150/</t>
+          <t>https://book.douban.com/subject/30231751/</t>
         </is>
       </c>
     </row>
@@ -9320,12 +9320,12 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>ONE-PUNCH MAN 一拳超人 11</t>
+          <t>ONE-PUNCH MAN 一拳超人 15</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2016-7-18 / NT$100</t>
+          <t>原作：ONE、漫畫：村田雄介 / 吳勵誠 / 東立出版社 / 2018-2-28 / NTD100</t>
         </is>
       </c>
       <c r="D253" s="2" t="n">
@@ -9342,7 +9342,7 @@
       <c r="G253" t="inlineStr"/>
       <c r="H253" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/26844477/</t>
+          <t>https://book.douban.com/subject/28461662/</t>
         </is>
       </c>
     </row>
@@ -9352,12 +9352,12 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>ONE-PUNCH MAN 一拳超人 05</t>
+          <t>ONE-PUNCH MAN 一拳超人 14</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2015-11-13 / NT$100</t>
+          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2018-10-3 / NT$100</t>
         </is>
       </c>
       <c r="D254" s="2" t="n">
@@ -9374,7 +9374,7 @@
       <c r="G254" t="inlineStr"/>
       <c r="H254" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/26429148/</t>
+          <t>https://book.douban.com/subject/27173099/</t>
         </is>
       </c>
     </row>
@@ -9384,12 +9384,12 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>ONE-PUNCH MAN 一拳超人 03</t>
+          <t>ONE-PUNCH MAN 一拳超人 13</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2015-10-8 / NT$100</t>
+          <t>原作：ONE、漫畫：村田雄介 / 吳勵誠 / 東立 / 2017-6-12 / NT100</t>
         </is>
       </c>
       <c r="D255" s="2" t="n">
@@ -9406,7 +9406,7 @@
       <c r="G255" t="inlineStr"/>
       <c r="H255" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/26429146/</t>
+          <t>https://book.douban.com/subject/27078222/</t>
         </is>
       </c>
     </row>
@@ -9416,12 +9416,12 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>ONE-PUNCH MAN 一拳超人 10</t>
+          <t>ONE-PUNCH MAN 一拳超人 12</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2016-2-25 / NT$100</t>
+          <t>ONE、村田雄介 / 吳勵誠 / 東立 / 2017-1-24 / NTD100</t>
         </is>
       </c>
       <c r="D256" s="2" t="n">
@@ -9438,7 +9438,7 @@
       <c r="G256" t="inlineStr"/>
       <c r="H256" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/26663170/</t>
+          <t>https://book.douban.com/subject/26971230/</t>
         </is>
       </c>
     </row>
@@ -9448,12 +9448,12 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>ONE-PUNCH MAN 一拳超人 01</t>
+          <t>ONE-PUNCH MAN 一拳超人 11</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2015-8-5 / NT$100</t>
+          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2016-7-18 / NT$100</t>
         </is>
       </c>
       <c r="D257" s="2" t="n">
@@ -9470,7 +9470,7 @@
       <c r="G257" t="inlineStr"/>
       <c r="H257" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/26429140/</t>
+          <t>https://book.douban.com/subject/26844477/</t>
         </is>
       </c>
     </row>
@@ -9480,12 +9480,12 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>ONE-PUNCH MAN 一拳超人 04</t>
+          <t>ONE-PUNCH MAN 一拳超人 01</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2015-10-30 / NT$100</t>
+          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2015-8-5 / NT$100</t>
         </is>
       </c>
       <c r="D258" s="2" t="n">
@@ -9502,7 +9502,7 @@
       <c r="G258" t="inlineStr"/>
       <c r="H258" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/26429147/</t>
+          <t>https://book.douban.com/subject/26429140/</t>
         </is>
       </c>
     </row>
@@ -9512,12 +9512,12 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>ONE-PUNCH MAN 一拳超人 13</t>
+          <t>ONE-PUNCH MAN 一拳超人 08</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>原作：ONE、漫畫：村田雄介 / 吳勵誠 / 東立 / 2017-6-12 / NT100</t>
+          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2016-1-29 / NT$100</t>
         </is>
       </c>
       <c r="D259" s="2" t="n">
@@ -9534,7 +9534,7 @@
       <c r="G259" t="inlineStr"/>
       <c r="H259" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/27078222/</t>
+          <t>https://book.douban.com/subject/26429151/</t>
         </is>
       </c>
     </row>
@@ -9544,12 +9544,12 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>ONE-PUNCH MAN 一拳超人 12</t>
+          <t>ONE-PUNCH MAN 一拳超人 02</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>ONE、村田雄介 / 吳勵誠 / 東立 / 2017-1-24 / NTD100</t>
+          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2015-9-2 / NT$100</t>
         </is>
       </c>
       <c r="D260" s="2" t="n">
@@ -9566,7 +9566,7 @@
       <c r="G260" t="inlineStr"/>
       <c r="H260" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/26971230/</t>
+          <t>https://book.douban.com/subject/26429145/</t>
         </is>
       </c>
     </row>
@@ -9576,12 +9576,12 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>ONE-PUNCH MAN 一拳超人 19</t>
+          <t>ONE-PUNCH MAN 一拳超人 03</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>ONE、村田雄介 / 吳勵誠 / 東立 / 2019-6-17 / NT$100</t>
+          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2015-10-8 / NT$100</t>
         </is>
       </c>
       <c r="D261" s="2" t="n">
@@ -9598,7 +9598,7 @@
       <c r="G261" t="inlineStr"/>
       <c r="H261" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/34434070/</t>
+          <t>https://book.douban.com/subject/26429146/</t>
         </is>
       </c>
     </row>
@@ -9608,12 +9608,12 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>ONE PUNCH MAN一拳超人 18</t>
+          <t>ONE-PUNCH MAN 一拳超人 04</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>村田雄介、ONE / 吳勵誠 / 東立出版社 / 2019-2-20 / NT100</t>
+          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2015-10-30 / NT$100</t>
         </is>
       </c>
       <c r="D262" s="2" t="n">
@@ -9630,7 +9630,7 @@
       <c r="G262" t="inlineStr"/>
       <c r="H262" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/30380122/</t>
+          <t>https://book.douban.com/subject/26429147/</t>
         </is>
       </c>
     </row>
@@ -9640,12 +9640,12 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>ONE PUNCH MAN一拳超人 17</t>
+          <t>ONE-PUNCH MAN 一拳超人 10</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2018-11-15 / NT100</t>
+          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2016-2-25 / NT$100</t>
         </is>
       </c>
       <c r="D263" s="2" t="n">
@@ -9662,7 +9662,7 @@
       <c r="G263" t="inlineStr"/>
       <c r="H263" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/30278079/</t>
+          <t>https://book.douban.com/subject/26663170/</t>
         </is>
       </c>
     </row>
@@ -9672,12 +9672,12 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>ONE-PUNCH MAN 一拳超人 02</t>
+          <t>ONE-PUNCH MAN 一拳超人 06</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2015-9-2 / NT$100</t>
+          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2015-12-2 / NT$100</t>
         </is>
       </c>
       <c r="D264" s="2" t="n">
@@ -9694,7 +9694,7 @@
       <c r="G264" t="inlineStr"/>
       <c r="H264" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/26429145/</t>
+          <t>https://book.douban.com/subject/26429149/</t>
         </is>
       </c>
     </row>
@@ -9704,12 +9704,12 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>ONE-PUNCH MAN 一拳超人 15</t>
+          <t>ONE-PUNCH MAN 一拳超人 09</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>原作：ONE、漫畫：村田雄介 / 吳勵誠 / 東立出版社 / 2018-2-28 / NTD100</t>
+          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2016-2-4 / NT$100</t>
         </is>
       </c>
       <c r="D265" s="2" t="n">
@@ -9726,7 +9726,7 @@
       <c r="G265" t="inlineStr"/>
       <c r="H265" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/28461662/</t>
+          <t>https://book.douban.com/subject/26577748/</t>
         </is>
       </c>
     </row>
@@ -9736,12 +9736,12 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>ONE-PUNCH MAN 一拳超人 14</t>
+          <t>ONE-PUNCH MAN 一拳超人 05</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2018-10-3 / NT$100</t>
+          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2015-11-13 / NT$100</t>
         </is>
       </c>
       <c r="D266" s="2" t="n">
@@ -9758,7 +9758,7 @@
       <c r="G266" t="inlineStr"/>
       <c r="H266" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/27173099/</t>
+          <t>https://book.douban.com/subject/26429148/</t>
         </is>
       </c>
     </row>
@@ -9768,12 +9768,12 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>ONE-PUNCH MAN 一拳超人 16</t>
+          <t>ONE-PUNCH MAN 一拳超人 07</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>ONE、村田雄介 / 吳勵誠 / 東立 / 2018-5-30 / NT$100</t>
+          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2015-12-21 / NT$100</t>
         </is>
       </c>
       <c r="D267" s="2" t="n">
@@ -9790,7 +9790,7 @@
       <c r="G267" t="inlineStr"/>
       <c r="H267" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/30231751/</t>
+          <t>https://book.douban.com/subject/26429150/</t>
         </is>
       </c>
     </row>
@@ -10584,33 +10584,33 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>商业模式新生代</t>
+          <t>深河</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>亚历山大•奥斯特瓦德 (Alexander Osterwalder)、伊夫•皮尼厄 (Yves Pigneur) / 王帅、毛心宇、严威 / 机械工业出版社 / 2011-8-15 / 88.00元</t>
+          <t>(日)远藤周作 / 林水福 / 南海出版公司 / 2013-5 / 36.00元</t>
         </is>
       </c>
       <c r="D290" s="2" t="n">
         <v>44165</v>
       </c>
       <c r="E290" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>应用书籍</t>
+          <t>日语文学 外国文学 #新经典</t>
         </is>
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>也算是，读完了...</t>
+          <t>四个不同的男女因为各自的原因来到恒河：寻找离世妻子的转世，看望因为异端信仰被教会驱逐的神甫大学同学，为死去的战友超度亡魂和放生自己坚信代替自己死去的一只鸟的同类。这是一条生与死交汇在一起的河流。这四个男女各自有各自的痛苦，但是恒河接纳他们，一如接纳高贵的婆罗门僧侣和低微的贱民。第二次读远藤周作的书，他的书带给我一种淡淡忧伤之感。和《沉默》一样，这本书将也设置了日本和海外的双重背景，通过外国人的言行和基督教信仰来反思日本人自己的思想和意识形态。不过读到小说里的三条夫妇时，不知道为什么竟然联想到了我们国家的一些人。看来狭隘的人什么时候，什么地方都有。</t>
         </is>
       </c>
       <c r="H290" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/6718487/</t>
+          <t>https://book.douban.com/subject/21692809/</t>
         </is>
       </c>
     </row>
@@ -10620,33 +10620,33 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>深河</t>
+          <t>商业模式新生代</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>(日)远藤周作 / 林水福 / 南海出版公司 / 2013-5 / 36.00元</t>
+          <t>亚历山大•奥斯特瓦德 (Alexander Osterwalder)、伊夫•皮尼厄 (Yves Pigneur) / 王帅、毛心宇、严威 / 机械工业出版社 / 2011-8-15 / 88.00元</t>
         </is>
       </c>
       <c r="D291" s="2" t="n">
         <v>44165</v>
       </c>
       <c r="E291" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>日语文学 外国文学 #新经典</t>
+          <t>应用书籍</t>
         </is>
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>四个不同的男女因为各自的原因来到恒河：寻找离世妻子的转世，看望因为异端信仰被教会驱逐的神甫大学同学，为死去的战友超度亡魂和放生自己坚信代替自己死去的一只鸟的同类。这是一条生与死交汇在一起的河流。这四个男女各自有各自的痛苦，但是恒河接纳他们，一如接纳高贵的婆罗门僧侣和低微的贱民。第二次读远藤周作的书，他的书带给我一种淡淡忧伤之感。和《沉默》一样，这本书将也设置了日本和海外的双重背景，通过外国人的言行和基督教信仰来反思日本人自己的思想和意识形态。不过读到小说里的三条夫妇时，不知道为什么竟然联想到了我们国家的一些人。看来狭隘的人什么时候，什么地方都有。</t>
+          <t>也算是，读完了...</t>
         </is>
       </c>
       <c r="H291" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/21692809/</t>
+          <t>https://book.douban.com/subject/6718487/</t>
         </is>
       </c>
     </row>
@@ -10800,19 +10800,19 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>巴黎圣母院</t>
+          <t>悲惨世界</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>维克多·雨果 / 陈敬容 / 人民文学出版社 / 1982-6 / 22.00元</t>
+          <t>雨果 / 李丹、方于 / 人民文学出版社 / 1992-6 / 70.00元</t>
         </is>
       </c>
       <c r="D296" s="2" t="n">
         <v>44193</v>
       </c>
       <c r="E296" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F296" t="inlineStr">
         <is>
@@ -10821,12 +10821,12 @@
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>P3:巴黎人被旧城区、大学区和市民区三重城垣里一片轰鸣的钟声惊醒的那个日子，距离今天已经有三百四十八年六个月零十九天了。这个开头似乎和现代派的某些小说有异曲同工之妙。P58:哲人的一生，他的命运老是攻击他的哲学。 副主教克洛德·孚罗洛是一个悲剧人物。一个终生被禁欲的男人，生理不健康心理怎么能健康？他因爱生恨，得不到的都想毁灭。也许常年的离群索居、独自研究造成了他阴沉孤僻的性格，但这并不是他泯灭人性，失去善良的理由。 弗比斯队长是个很市井的人，他空有一个外表，其他什么都没有。最后雨果给他的结局很耐人寻味：“弗比斯·德·沙多倍尔也得到了一个悲剧的收场：他结婚了”。而卡西莫多，他看着爱斯梅拉达和克洛德的一句话“啊！都是我爱过的人呀！”是多么心酸。P222：雨果关于女人嫉妒的言论。</t>
+          <t>P935: 一个女人来到你的跟前，一面走，一面放光，从那时起，你便完了，你便爱了。你只有一条路可走，集中全部力量去想她，以迫使她也来想你。 冉阿让是卞汝福主教生命的延续，书中花一卷的笔墨写他教想必就是为了铺垫他高尚的性格足以改变任何一个人。珂赛特和爱潘妮相比，我更喜欢后者。尤其是最后那句话“我想我从一开始就有些爱你呢。”道尽了人世单相思之苦。整本书情感铺垫很到位，只是额外描写太多，多荡开一笔，使得小说有些冗长，如同塞满家具的房间，每个木器都是精雕细刻，可是房间太满，没有转身的空间。这恐怕是所有史诗的弊端吧。</t>
         </is>
       </c>
       <c r="H296" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/3181275/</t>
+          <t>https://book.douban.com/subject/3200760/</t>
         </is>
       </c>
     </row>
@@ -10836,33 +10836,33 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>斯·茨威格中短篇小说选</t>
+          <t>巴黎圣母院</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>斯·茨威格 / 张玉书 / 人民文学出版社 / 2006-6-1 / 24.00元</t>
+          <t>维克多·雨果 / 陈敬容 / 人民文学出版社 / 1982-6 / 22.00元</t>
         </is>
       </c>
       <c r="D297" s="2" t="n">
         <v>44193</v>
       </c>
       <c r="E297" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>#人民文学 外国文学 德语文学</t>
+          <t>#人民文学 外国文学 法语文学</t>
         </is>
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>这本书中，我最喜欢《一个陌生女人的来信》和《无形的压力》。茨威格不愧是心理描写大师。他往往用第一人称叙述故事的方法来表现人物的内心。他的故事没有卡夫卡的荒诞不经，也没有契诃夫的沉重忧郁，而是有他自己风格的奇闻异事，但是他又将自己对这些角色的同情注入作品中，使其充满人道主义色彩。</t>
+          <t>P3:巴黎人被旧城区、大学区和市民区三重城垣里一片轰鸣的钟声惊醒的那个日子，距离今天已经有三百四十八年六个月零十九天了。这个开头似乎和现代派的某些小说有异曲同工之妙。P58:哲人的一生，他的命运老是攻击他的哲学。 副主教克洛德·孚罗洛是一个悲剧人物。一个终生被禁欲的男人，生理不健康心理怎么能健康？他因爱生恨，得不到的都想毁灭。也许常年的离群索居、独自研究造成了他阴沉孤僻的性格，但这并不是他泯灭人性，失去善良的理由。 弗比斯队长是个很市井的人，他空有一个外表，其他什么都没有。最后雨果给他的结局很耐人寻味：“弗比斯·德·沙多倍尔也得到了一个悲剧的收场：他结婚了”。而卡西莫多，他看着爱斯梅拉达和克洛德的一句话“啊！都是我爱过的人呀！”是多么心酸。P222：雨果关于女人嫉妒的言论。</t>
         </is>
       </c>
       <c r="H297" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/3200730/</t>
+          <t>https://book.douban.com/subject/3181275/</t>
         </is>
       </c>
     </row>
@@ -10940,33 +10940,33 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>格列佛游记</t>
+          <t>契诃夫短篇小说选</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>乔纳森·斯威夫特 / 张健 / 人民文学出版社 / 1979-12 / 16.00元</t>
+          <t>契诃夫 / 汝龙 / 人民文学出版社 / 2002-6 / 15.00元</t>
         </is>
       </c>
       <c r="D300" s="2" t="n">
         <v>44193</v>
       </c>
       <c r="E300" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>#人民文学 英语文学 外国文学</t>
+          <t>#人民文学 俄语文学 外国文学</t>
         </is>
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>初中时候读的，有些情节其实非常重口......</t>
+          <t>有些沉重，尤其是在发现他所写的现象今日在身边还存在时。</t>
         </is>
       </c>
       <c r="H300" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/3181278/</t>
+          <t>https://book.douban.com/subject/3181280/</t>
         </is>
       </c>
     </row>
@@ -10976,12 +10976,12 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>鲁滨孙飘流记</t>
+          <t>格列佛游记</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>丹尼尔•笛福 / 徐霞村 / 人民文学出版社 / 1959-9-1 / 15.00元</t>
+          <t>乔纳森·斯威夫特 / 张健 / 人民文学出版社 / 1979-12 / 16.00元</t>
         </is>
       </c>
       <c r="D301" s="2" t="n">
@@ -10997,12 +10997,12 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>记得还是初中时候读的，现在明白为什么自己对建造类的游戏那么感兴趣了......</t>
+          <t>初中时候读的，有些情节其实非常重口......</t>
         </is>
       </c>
       <c r="H301" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/3200739/</t>
+          <t>https://book.douban.com/subject/3181278/</t>
         </is>
       </c>
     </row>
@@ -11012,33 +11012,33 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>悲惨世界</t>
+          <t>鲁滨孙飘流记</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>雨果 / 李丹、方于 / 人民文学出版社 / 1992-6 / 70.00元</t>
+          <t>丹尼尔•笛福 / 徐霞村 / 人民文学出版社 / 1959-9-1 / 15.00元</t>
         </is>
       </c>
       <c r="D302" s="2" t="n">
         <v>44193</v>
       </c>
       <c r="E302" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F302" t="inlineStr">
         <is>
-          <t>#人民文学 外国文学 法语文学</t>
+          <t>#人民文学 英语文学 外国文学</t>
         </is>
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>P935: 一个女人来到你的跟前，一面走，一面放光，从那时起，你便完了，你便爱了。你只有一条路可走，集中全部力量去想她，以迫使她也来想你。 冉阿让是卞汝福主教生命的延续，书中花一卷的笔墨写他教想必就是为了铺垫他高尚的性格足以改变任何一个人。珂赛特和爱潘妮相比，我更喜欢后者。尤其是最后那句话“我想我从一开始就有些爱你呢。”道尽了人世单相思之苦。整本书情感铺垫很到位，只是额外描写太多，多荡开一笔，使得小说有些冗长，如同塞满家具的房间，每个木器都是精雕细刻，可是房间太满，没有转身的空间。这恐怕是所有史诗的弊端吧。</t>
+          <t>记得还是初中时候读的，现在明白为什么自己对建造类的游戏那么感兴趣了......</t>
         </is>
       </c>
       <c r="H302" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/3200760/</t>
+          <t>https://book.douban.com/subject/3200739/</t>
         </is>
       </c>
     </row>
@@ -11048,33 +11048,33 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>契诃夫短篇小说选</t>
+          <t>斯·茨威格中短篇小说选</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>契诃夫 / 汝龙 / 人民文学出版社 / 2002-6 / 15.00元</t>
+          <t>斯·茨威格 / 张玉书 / 人民文学出版社 / 2006-6-1 / 24.00元</t>
         </is>
       </c>
       <c r="D303" s="2" t="n">
         <v>44193</v>
       </c>
       <c r="E303" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>#人民文学 俄语文学 外国文学</t>
+          <t>#人民文学 外国文学 德语文学</t>
         </is>
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>有些沉重，尤其是在发现他所写的现象今日在身边还存在时。</t>
+          <t>这本书中，我最喜欢《一个陌生女人的来信》和《无形的压力》。茨威格不愧是心理描写大师。他往往用第一人称叙述故事的方法来表现人物的内心。他的故事没有卡夫卡的荒诞不经，也没有契诃夫的沉重忧郁，而是有他自己风格的奇闻异事，但是他又将自己对这些角色的同情注入作品中，使其充满人道主义色彩。</t>
         </is>
       </c>
       <c r="H303" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/3181280/</t>
+          <t>https://book.douban.com/subject/3200730/</t>
         </is>
       </c>
     </row>
@@ -11300,12 +11300,12 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>皮德漫画</t>
+          <t>1844年经济学哲学手稿</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>［丹麦］皮德斯特鲁普 / 译林出版社 / 2018-12 / 68.00元</t>
+          <t>[德] 卡尔·马克思 / 中共中央马克思恩格斯列宁斯大林著作编译局 / 人民出版社 / 2018-4-1 / 48.00元</t>
         </is>
       </c>
       <c r="D310" s="2" t="n">
@@ -11316,17 +11316,17 @@
       </c>
       <c r="F310" t="inlineStr">
         <is>
-          <t>绘本</t>
+          <t>社会科学</t>
         </is>
       </c>
       <c r="G310" t="inlineStr">
         <is>
-          <t>就是这种漫画，小时候读过好多，时而讽刺时而温馨......</t>
+          <t>当初是因为想更加了解目前的社会问题才买了这本书，读完之后发现马克思对整个资本主义社会的发展进行了阐释。虽然只是手稿，但是第一部分的论证仍然十分清晰，按资本，地租，异化劳动三个方面来阐述工人阶级的生存难题。可惜的是我所学尚浅，第二、第三部分的哲学部分都因为读不懂跳过了。不过在这本书里，马克思还在解释问题，关于具体怎么解决这个问题并没有探讨。巧合的是读到这本书的同时在读卡夫卡的《城堡》，一个从社会学角度论证人的异化，一个从文学角度论证人的异化，读起来让人不寒而栗。</t>
         </is>
       </c>
       <c r="H310" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/30232121/</t>
+          <t>https://book.douban.com/subject/30153583/</t>
         </is>
       </c>
     </row>
@@ -11336,12 +11336,12 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>1844年经济学哲学手稿</t>
+          <t>皮德漫画</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>[德] 卡尔·马克思 / 中共中央马克思恩格斯列宁斯大林著作编译局 / 人民出版社 / 2018-4-1 / 48.00元</t>
+          <t>［丹麦］皮德斯特鲁普 / 译林出版社 / 2018-12 / 68.00元</t>
         </is>
       </c>
       <c r="D311" s="2" t="n">
@@ -11352,17 +11352,17 @@
       </c>
       <c r="F311" t="inlineStr">
         <is>
-          <t>社会科学</t>
+          <t>绘本</t>
         </is>
       </c>
       <c r="G311" t="inlineStr">
         <is>
-          <t>当初是因为想更加了解目前的社会问题才买了这本书，读完之后发现马克思对整个资本主义社会的发展进行了阐释。虽然只是手稿，但是第一部分的论证仍然十分清晰，按资本，地租，异化劳动三个方面来阐述工人阶级的生存难题。可惜的是我所学尚浅，第二、第三部分的哲学部分都因为读不懂跳过了。不过在这本书里，马克思还在解释问题，关于具体怎么解决这个问题并没有探讨。巧合的是读到这本书的同时在读卡夫卡的《城堡》，一个从社会学角度论证人的异化，一个从文学角度论证人的异化，读起来让人不寒而栗。</t>
+          <t>就是这种漫画，小时候读过好多，时而讽刺时而温馨......</t>
         </is>
       </c>
       <c r="H311" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/30153583/</t>
+          <t>https://book.douban.com/subject/30232121/</t>
         </is>
       </c>
     </row>
@@ -11696,12 +11696,12 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>ONE-PUNCH MAN 一拳超人 22</t>
+          <t>斯泰尔斯庄园奇案</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2021-1-14 / NT$100</t>
+          <t>(英)阿加莎·克里斯蒂 / 郑卫明 / 新星出版社 / 2013-3 / 28.00元</t>
         </is>
       </c>
       <c r="D321" s="2" t="n">
@@ -11712,13 +11712,17 @@
       </c>
       <c r="F321" t="inlineStr">
         <is>
-          <t>绘本</t>
-        </is>
-      </c>
-      <c r="G321" t="inlineStr"/>
+          <t>外国文学 侦探小说 英语文学</t>
+        </is>
+      </c>
+      <c r="G321" t="inlineStr">
+        <is>
+          <t>“坚持自己的权利常常也是一个人的责任。”又是关于遗产的谋杀案，看来太有钱也是个危险的信号......</t>
+        </is>
+      </c>
       <c r="H321" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/35128227/</t>
+          <t>https://book.douban.com/subject/21692860/</t>
         </is>
       </c>
     </row>
@@ -11728,12 +11732,12 @@
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>斯泰尔斯庄园奇案</t>
+          <t>ONE-PUNCH MAN 一拳超人 22</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>(英)阿加莎·克里斯蒂 / 郑卫明 / 新星出版社 / 2013-3 / 28.00元</t>
+          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2021-1-14 / NT$100</t>
         </is>
       </c>
       <c r="D322" s="2" t="n">
@@ -11744,17 +11748,13 @@
       </c>
       <c r="F322" t="inlineStr">
         <is>
-          <t>外国文学 侦探小说 英语文学</t>
-        </is>
-      </c>
-      <c r="G322" t="inlineStr">
-        <is>
-          <t>“坚持自己的权利常常也是一个人的责任。”又是关于遗产的谋杀案，看来太有钱也是个危险的信号......</t>
-        </is>
-      </c>
+          <t>绘本</t>
+        </is>
+      </c>
+      <c r="G322" t="inlineStr"/>
       <c r="H322" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/21692860/</t>
+          <t>https://book.douban.com/subject/35128227/</t>
         </is>
       </c>
     </row>
@@ -11800,33 +11800,33 @@
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>茶馆</t>
+          <t>追寻逝去的时光</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>老舍著、叶浅予绘 / 人民文学出版社 / 2016-1-1 / 19</t>
+          <t>[法] 马塞尔·普鲁斯特 / 周克希 / 华东师范大学出版社 / 2019-8 / 88.00元</t>
         </is>
       </c>
       <c r="D324" s="2" t="n">
         <v>44316</v>
       </c>
       <c r="E324" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F324" t="inlineStr">
         <is>
-          <t>汉语文学 现当代文学</t>
+          <t>#周克希译文集 外国文学 法语文学</t>
         </is>
       </c>
       <c r="G324" t="inlineStr">
         <is>
-          <t>当年本科在上20世纪的中国文学时读的。我想老舍先生在遣词造句方面下的功夫是极大的吧。原汁原味的北京话，再现了一个世纪之前的北京。只是我觉得老舍先生所批判的是特定的社会（晚晴和民国初年）对当时平凡人的迫害，但是没有将其上升到对国民本身缺点的批判。从这点上来说，《茶馆》受到了其时代局限性。</t>
+          <t>从贡布雷的玛德莱纳小蛋糕，睡觉前妈妈的吻，巴尔贝克的三棵树在七部中反复出现，到在最后一部中斯万家和盖尔芒特家错综复杂的关系延续到圣卢小姐身上完成一种和谐的统一，普鲁斯特用人生最后二十年写就的这本书，仿佛一座宏伟的时光大教堂，哪怕在最无人注意的细节都令人啧啧称奇。“在这个世界上尽管万物都会衰退，万物都会消亡，却有一样东西，它和美相比，销毁得更彻底，而留下的痕迹更少：那就是悲伤”在经过人事无常的洗礼后，书中的主角终于明白，只有写出包容自己过去的作品，才能封存那些美好的时光。所以，我们看见了音乐（第一部中凡特伊的奏鸣曲），看见了绘画（第二部中埃尔斯蒂尔模仿夏尔丹的绘画），看见了文学（第五部中与阿尔贝蒂娜谈论陀思妥耶夫斯基），最重要的是，也看见了过去的那些活生生的人。谢谢普鲁斯特，谢谢周克希先生。</t>
         </is>
       </c>
       <c r="H324" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/26816586/</t>
+          <t>https://book.douban.com/subject/33395271/</t>
         </is>
       </c>
     </row>
@@ -11836,19 +11836,19 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>彷徨</t>
+          <t>呐喊</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>鲁迅 / 译林出版社 / 2013-11 / 12.8元</t>
+          <t>鲁迅 / 译林出版社 / 2013-11-1 / 10.8</t>
         </is>
       </c>
       <c r="D325" s="2" t="n">
         <v>44316</v>
       </c>
       <c r="E325" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F325" t="inlineStr">
         <is>
@@ -11857,12 +11857,12 @@
       </c>
       <c r="G325" t="inlineStr">
         <is>
-          <t>当年本科在上20世纪的中国文学时读的。记得放关于鲁迅的纪录片，还提到了魏连殳。想想书里说到他，还说读过《沉沦》，真是和郁达夫奇妙的联动。像是魏连殳这样的孤独者，今天会怎么样呢？</t>
+          <t>说实话，想想以前小时候不喜欢鲁迅还真是挺脸红的。如果现在让我选最喜欢的中国作家，我还是会选鲁迅的。以前小时候很鄙视一些大人才有的行为，没想到自己长大后却成了一样的大人。读鲁迅的小说，就像看见腐败的自己一样， 虽然难受，但是终究是意识到了自己有问题。而意识到自己的问题，就是解决问题的第一步。</t>
         </is>
       </c>
       <c r="H325" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/25778492/</t>
+          <t>https://book.douban.com/subject/25745773/</t>
         </is>
       </c>
     </row>
@@ -11872,33 +11872,33 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>追寻逝去的时光</t>
+          <t>彷徨</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>[法] 马塞尔·普鲁斯特 / 周克希 / 华东师范大学出版社 / 2019-8 / 88.00元</t>
+          <t>鲁迅 / 译林出版社 / 2013-11 / 12.8元</t>
         </is>
       </c>
       <c r="D326" s="2" t="n">
         <v>44316</v>
       </c>
       <c r="E326" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F326" t="inlineStr">
         <is>
-          <t>#周克希译文集 外国文学 法语文学</t>
+          <t>现当代文学 汉语文学</t>
         </is>
       </c>
       <c r="G326" t="inlineStr">
         <is>
-          <t>从贡布雷的玛德莱纳小蛋糕，睡觉前妈妈的吻，巴尔贝克的三棵树在七部中反复出现，到在最后一部中斯万家和盖尔芒特家错综复杂的关系延续到圣卢小姐身上完成一种和谐的统一，普鲁斯特用人生最后二十年写就的这本书，仿佛一座宏伟的时光大教堂，哪怕在最无人注意的细节都令人啧啧称奇。“在这个世界上尽管万物都会衰退，万物都会消亡，却有一样东西，它和美相比，销毁得更彻底，而留下的痕迹更少：那就是悲伤”在经过人事无常的洗礼后，书中的主角终于明白，只有写出包容自己过去的作品，才能封存那些美好的时光。所以，我们看见了音乐（第一部中凡特伊的奏鸣曲），看见了绘画（第二部中埃尔斯蒂尔模仿夏尔丹的绘画），看见了文学（第五部中与阿尔贝蒂娜谈论陀思妥耶夫斯基），最重要的是，也看见了过去的那些活生生的人。谢谢普鲁斯特，谢谢周克希先生。</t>
+          <t>当年本科在上20世纪的中国文学时读的。记得放关于鲁迅的纪录片，还提到了魏连殳。想想书里说到他，还说读过《沉沦》，真是和郁达夫奇妙的联动。像是魏连殳这样的孤独者，今天会怎么样呢？</t>
         </is>
       </c>
       <c r="H326" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/33395271/</t>
+          <t>https://book.douban.com/subject/25778492/</t>
         </is>
       </c>
     </row>
@@ -11908,33 +11908,33 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>呐喊</t>
+          <t>茶馆</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>鲁迅 / 译林出版社 / 2013-11-1 / 10.8</t>
+          <t>老舍著、叶浅予绘 / 人民文学出版社 / 2016-1-1 / 19</t>
         </is>
       </c>
       <c r="D327" s="2" t="n">
         <v>44316</v>
       </c>
       <c r="E327" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F327" t="inlineStr">
         <is>
-          <t>现当代文学 汉语文学</t>
+          <t>汉语文学 现当代文学</t>
         </is>
       </c>
       <c r="G327" t="inlineStr">
         <is>
-          <t>说实话，想想以前小时候不喜欢鲁迅还真是挺脸红的。如果现在让我选最喜欢的中国作家，我还是会选鲁迅的。以前小时候很鄙视一些大人才有的行为，没想到自己长大后却成了一样的大人。读鲁迅的小说，就像看见腐败的自己一样， 虽然难受，但是终究是意识到了自己有问题。而意识到自己的问题，就是解决问题的第一步。</t>
+          <t>当年本科在上20世纪的中国文学时读的。我想老舍先生在遣词造句方面下的功夫是极大的吧。原汁原味的北京话，再现了一个世纪之前的北京。只是我觉得老舍先生所批判的是特定的社会（晚晴和民国初年）对当时平凡人的迫害，但是没有将其上升到对国民本身缺点的批判。从这点上来说，《茶馆》受到了其时代局限性。</t>
         </is>
       </c>
       <c r="H327" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/25745773/</t>
+          <t>https://book.douban.com/subject/26816586/</t>
         </is>
       </c>
     </row>
@@ -12845,7 +12845,7 @@
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>陀思妥耶夫斯基 (Ф.М.Достоевский) / 荣如德 / 上海译文出版社 / 2015-2-1 / CNY 78.00</t>
+          <t>[俄] 费奥多尔·陀思妥耶夫斯基 / 荣如德 / 上海译文出版社 / 2015-2-1 / CNY 78.00</t>
         </is>
       </c>
       <c r="D353" s="2" t="n">
@@ -12948,29 +12948,33 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>唐诗三百首</t>
+          <t>俗世奇人·贰</t>
         </is>
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>蘅塘退士 编 / 四川文艺出版社 / 2008-1 / 11.00元</t>
+          <t>冯骥才 / 有2016年7月10印本 / 作家出版社 / 2015-11 / 22.00元</t>
         </is>
       </c>
       <c r="D356" s="2" t="n">
         <v>44561</v>
       </c>
       <c r="E356" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F356" t="inlineStr">
         <is>
-          <t>汉语文学 古典文学 诗歌</t>
-        </is>
-      </c>
-      <c r="G356" t="inlineStr"/>
+          <t>汉语文学 现当代文学</t>
+        </is>
+      </c>
+      <c r="G356" t="inlineStr">
+        <is>
+          <t>原来我还读过这本书，不过没什么印象了...</t>
+        </is>
+      </c>
       <c r="H356" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/2987738/</t>
+          <t>https://book.douban.com/subject/26663303/</t>
         </is>
       </c>
     </row>
@@ -12980,33 +12984,29 @@
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>俗世奇人·贰</t>
+          <t>唐诗三百首</t>
         </is>
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>冯骥才 / 有2016年7月10印本 / 作家出版社 / 2015-11 / 22.00元</t>
+          <t>蘅塘退士 编 / 四川文艺出版社 / 2008-1 / 11.00元</t>
         </is>
       </c>
       <c r="D357" s="2" t="n">
         <v>44561</v>
       </c>
       <c r="E357" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F357" t="inlineStr">
         <is>
-          <t>汉语文学 现当代文学</t>
-        </is>
-      </c>
-      <c r="G357" t="inlineStr">
-        <is>
-          <t>原来我还读过这本书，不过没什么印象了...</t>
-        </is>
-      </c>
+          <t>汉语文学 古典文学 诗歌</t>
+        </is>
+      </c>
+      <c r="G357" t="inlineStr"/>
       <c r="H357" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/26663303/</t>
+          <t>https://book.douban.com/subject/2987738/</t>
         </is>
       </c>
     </row>
@@ -13880,12 +13880,12 @@
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>爱你的一万种方式</t>
+          <t>飞狐外传（全二册）</t>
         </is>
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>[美国] 莉兹·克里莫 / 七英俊 / 上海文艺出版社 / 2022-5 / 49.8</t>
+          <t>金庸 / 广州出版社 花城出版社 / 2008-3 / 41.00元</t>
         </is>
       </c>
       <c r="D382" s="2" t="n">
@@ -13896,17 +13896,17 @@
       </c>
       <c r="F382" t="inlineStr">
         <is>
-          <t>绘本</t>
+          <t>汉语文学 现当代文学 武侠小说</t>
         </is>
       </c>
       <c r="G382" t="inlineStr">
         <is>
-          <t>“日子仿佛很长，其实转瞬即逝。记得要停下来好好体会。因为在所有的欢笑，与泪水之间，那些无所事事的日常，那些值得纪念的日子，都是充满魔力的小小时光。你会记住它们的。”</t>
+          <t>说实话，我对《飞狐外传》是挺偏爱的。首先，这本书补充了许多关于《雪山飞狐》的细节（八卦门商家堡的复仇，胡一刀所中“毒手药王”之毒的来历，苗人凤和南兰的过去，两个武功奇怪的孩子的由来等），还顺便交代了《书剑恩仇录》的一些人物的（红花会群雄和福康安），给读者一种找彩蛋的快乐。此外，《雪》中个性并不鲜明的胡斐到了这本书终于变得面目清晰起来：比郭靖多了三分灵动，又比乔峰多了三分活泼，是个有些莽撞，但是急人所难的侠士。虽然有个金庸小说中最不受人待见的女主角袁紫衣，但好在程灵素足够出彩，连这个缺点也盖过了（不过袁紫衣的出家和程灵素的死真的是剧情杀，否则《雪》中的胡斐就彻底成了渣男）。只可惜了那个眼睛像漆一般黑的小姑娘再也种不了七星海棠了——“借如生死别，安得长苦悲”。</t>
         </is>
       </c>
       <c r="H382" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/35931636/</t>
+          <t>https://book.douban.com/subject/1212909/</t>
         </is>
       </c>
     </row>
@@ -13916,12 +13916,12 @@
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>飞狐外传（全二册）</t>
+          <t>爱你的一万种方式</t>
         </is>
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>金庸 / 广州出版社 花城出版社 / 2008-3 / 41.00元</t>
+          <t>[美国] 莉兹·克里莫 / 七英俊 / 上海文艺出版社 / 2022-5 / 49.8</t>
         </is>
       </c>
       <c r="D383" s="2" t="n">
@@ -13932,17 +13932,17 @@
       </c>
       <c r="F383" t="inlineStr">
         <is>
-          <t>汉语文学 现当代文学 武侠小说</t>
+          <t>绘本</t>
         </is>
       </c>
       <c r="G383" t="inlineStr">
         <is>
-          <t>说实话，我对《飞狐外传》是挺偏爱的。首先，这本书补充了许多关于《雪山飞狐》的细节（八卦门商家堡的复仇，胡一刀所中“毒手药王”之毒的来历，苗人凤和南兰的过去，两个武功奇怪的孩子的由来等），还顺便交代了《书剑恩仇录》的一些人物的（红花会群雄和福康安），给读者一种找彩蛋的快乐。此外，《雪》中个性并不鲜明的胡斐到了这本书终于变得面目清晰起来：比郭靖多了三分灵动，又比乔峰多了三分活泼，是个有些莽撞，但是急人所难的侠士。虽然有个金庸小说中最不受人待见的女主角袁紫衣，但好在程灵素足够出彩，连这个缺点也盖过了（不过袁紫衣的出家和程灵素的死真的是剧情杀，否则《雪》中的胡斐就彻底成了渣男）。只可惜了那个眼睛像漆一般黑的小姑娘再也种不了七星海棠了——“借如生死别，安得长苦悲”。</t>
+          <t>“日子仿佛很长，其实转瞬即逝。记得要停下来好好体会。因为在所有的欢笑，与泪水之间，那些无所事事的日常，那些值得纪念的日子，都是充满魔力的小小时光。你会记住它们的。”</t>
         </is>
       </c>
       <c r="H383" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/1212909/</t>
+          <t>https://book.douban.com/subject/35931636/</t>
         </is>
       </c>
     </row>
@@ -14708,33 +14708,33 @@
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>气球上的五星期</t>
+          <t>The Waste Land, Prufrock and Other Poems</t>
         </is>
       </c>
       <c r="C405" t="inlineStr">
         <is>
-          <t>儒勒·凡尔纳 / 曹剑 / 上海百家出版社 / 2009-1 / 28.00元</t>
+          <t>Eliot, T. S. / 2005-1 / $ 5.64</t>
         </is>
       </c>
       <c r="D405" s="2" t="n">
         <v>44913</v>
       </c>
       <c r="E405" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F405" t="inlineStr">
         <is>
-          <t>外国文学 法语文学 科幻小说</t>
+          <t>外国文学 英语文学 原版 诗歌</t>
         </is>
       </c>
       <c r="G405" t="inlineStr">
         <is>
-          <t>这一本居然是以三个英国人作为主角的，只有一个法国传教士，不过只登场了两章。现在想想这种书应该不算科幻小说了，而是冒险小说。如果书里的热气球方法可行，那再稍加改进一下——比如把气球做得结石一点，不怕鸟——是不是就可以靠着环球飞行了？我曾经听说过一句话：帆船是世界上最浪漫的交通方式，因为理论上只要有水的地方就能去，而地球70%的面积都是海洋。这么想，热气球才是最浪漫的交通方式，因为可以飞过整个地球。</t>
+          <t>"Nam Sibyllam quidem Cumis ego ipse oculis meis vidi in ampulla pendere, et cum illi pueri dicerent:Sibylla ti theleis; respondebat illa: apothanein thelo."是的，我自己亲眼看见古米的西比尔吊在一个笼子里。孩子们在问她：西比尔，你要什么，她回答说，我要死。Looking into the heart of light, the silence.Oed’ und leer das Meer.看进光的中心，那一片沉寂。荒凉而空虚是那大海。（真的读不懂）</t>
         </is>
       </c>
       <c r="H405" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/3527766/</t>
+          <t>https://book.douban.com/subject/7904472/</t>
         </is>
       </c>
     </row>
@@ -14744,33 +14744,33 @@
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>The Waste Land, Prufrock and Other Poems</t>
+          <t>气球上的五星期</t>
         </is>
       </c>
       <c r="C406" t="inlineStr">
         <is>
-          <t>Eliot, T. S. / 2005-1 / $ 5.64</t>
+          <t>儒勒·凡尔纳 / 曹剑 / 上海百家出版社 / 2009-1 / 28.00元</t>
         </is>
       </c>
       <c r="D406" s="2" t="n">
         <v>44913</v>
       </c>
       <c r="E406" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F406" t="inlineStr">
         <is>
-          <t>外国文学 英语文学 原版 诗歌</t>
+          <t>外国文学 法语文学 科幻小说</t>
         </is>
       </c>
       <c r="G406" t="inlineStr">
         <is>
-          <t>"Nam Sibyllam quidem Cumis ego ipse oculis meis vidi in ampulla pendere, et cum illi pueri dicerent:Sibylla ti theleis; respondebat illa: apothanein thelo."是的，我自己亲眼看见古米的西比尔吊在一个笼子里。孩子们在问她：西比尔，你要什么，她回答说，我要死。Looking into the heart of light, the silence.Oed’ und leer das Meer.看进光的中心，那一片沉寂。荒凉而空虚是那大海。（真的读不懂）</t>
+          <t>这一本居然是以三个英国人作为主角的，只有一个法国传教士，不过只登场了两章。现在想想这种书应该不算科幻小说了，而是冒险小说。如果书里的热气球方法可行，那再稍加改进一下——比如把气球做得结石一点，不怕鸟——是不是就可以靠着环球飞行了？我曾经听说过一句话：帆船是世界上最浪漫的交通方式，因为理论上只要有水的地方就能去，而地球70%的面积都是海洋。这么想，热气球才是最浪漫的交通方式，因为可以飞过整个地球。</t>
         </is>
       </c>
       <c r="H406" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/7904472/</t>
+          <t>https://book.douban.com/subject/3527766/</t>
         </is>
       </c>
     </row>
@@ -15068,19 +15068,19 @@
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>ONE-PUNCH MAN 一拳超人 27</t>
+          <t>ONE-PUNCH MAN 一拳超人 26</t>
         </is>
       </c>
       <c r="C415" t="inlineStr">
         <is>
-          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2023-5-26 / NT$110</t>
+          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2023-2-17 / NT$105</t>
         </is>
       </c>
       <c r="D415" s="2" t="n">
         <v>44983</v>
       </c>
       <c r="E415" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F415" t="inlineStr">
         <is>
@@ -15090,7 +15090,7 @@
       <c r="G415" t="inlineStr"/>
       <c r="H415" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/36210869/</t>
+          <t>https://book.douban.com/subject/35924557/</t>
         </is>
       </c>
     </row>
@@ -15100,19 +15100,19 @@
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>ONE-PUNCH MAN 一拳超人 24</t>
+          <t>ONE-PUNCH MAN 一拳超人 27</t>
         </is>
       </c>
       <c r="C416" t="inlineStr">
         <is>
-          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2022-4-14 / NT$105</t>
+          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2023-5-26 / NT$110</t>
         </is>
       </c>
       <c r="D416" s="2" t="n">
         <v>44983</v>
       </c>
       <c r="E416" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F416" t="inlineStr">
         <is>
@@ -15122,7 +15122,7 @@
       <c r="G416" t="inlineStr"/>
       <c r="H416" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/35690075/</t>
+          <t>https://book.douban.com/subject/36210869/</t>
         </is>
       </c>
     </row>
@@ -15132,12 +15132,12 @@
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>ONE-PUNCH MAN 一拳超人 25</t>
+          <t>ONE-PUNCH MAN 一拳超人 24</t>
         </is>
       </c>
       <c r="C417" t="inlineStr">
         <is>
-          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2022-12-15 / NT$105</t>
+          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2022-4-14 / NT$105</t>
         </is>
       </c>
       <c r="D417" s="2" t="n">
@@ -15154,7 +15154,7 @@
       <c r="G417" t="inlineStr"/>
       <c r="H417" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/35887927/</t>
+          <t>https://book.douban.com/subject/35690075/</t>
         </is>
       </c>
     </row>
@@ -15164,12 +15164,12 @@
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>ONE-PUNCH MAN 一拳超人 26</t>
+          <t>ONE-PUNCH MAN 一拳超人 25</t>
         </is>
       </c>
       <c r="C418" t="inlineStr">
         <is>
-          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2023-2-17 / NT$105</t>
+          <t>ONE、村田雄介 / 吳勵誠 / 東立出版社 / 2022-12-15 / NT$105</t>
         </is>
       </c>
       <c r="D418" s="2" t="n">
@@ -15186,7 +15186,7 @@
       <c r="G418" t="inlineStr"/>
       <c r="H418" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/35924557/</t>
+          <t>https://book.douban.com/subject/35887927/</t>
         </is>
       </c>
     </row>
@@ -15772,12 +15772,12 @@
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>李尔王</t>
+          <t>第十二夜</t>
         </is>
       </c>
       <c r="C435" t="inlineStr">
         <is>
-          <t>[英] 威廉·莎士比亚 / 朱生豪 / 译林出版社 / 39.80元</t>
+          <t>朱生豪 / 译林出版社 / 35.90元</t>
         </is>
       </c>
       <c r="D435" s="2" t="n">
@@ -15793,12 +15793,12 @@
       </c>
       <c r="G435" t="inlineStr">
         <is>
-          <t>如果说麦克白的悲剧是主人公的野心在预言和妻子的诱导下导致的咎由自取，奥赛罗的悲剧是主人公的冲动易怒的脾气和受小人蒙蔽的结果，那李尔王的悲剧就是李尔王作为一个父亲缺乏对女儿们的管教与了解导致的。“疯子带着瞎子走路，本来是这时代的一般病态。”，李尔王可以说既是疯子也是瞎子：他把自己所有的一切都交给了女儿们，而又没有交给真正最爱他的那个女儿。最后被两个利欲熏心的女儿敲骨吸髓，没能善终。李尔王的故事总让我想起电视里看到的那些晚景凄惨的老人：他们自己的孩子住在很好的房屋中，他们却只能在破旧的地方瑟瑟发抖。不过最让人伤心的还是格洛斯特：一个这么正直忠心的仆人，最后却落得了瞎眼身死的下场。</t>
+          <t>“别以为我这样向你求情，你就可以无须再献殷勤；须知求得的爱虽费心力，不劳而获的更应该珍惜。”威尼斯商人&amp;gt;无事生非&amp;gt;第十二夜&amp;gt;仲夏夜之梦。读的时候有好几次都有这样的感觉：为什么薇奥拉不直接表明自己的身份，亦或是听见有人错认自己的时候就直接拉着那个人问个清楚或去找自己的哥哥。如果这么干，这本书估计写到三分之一就结束了。结尾实在过于仓促了，当奥西诺被奥丽维娅拒绝且得知薇奥拉的真实身份之后，他居然立刻移情别恋，爱上了薇奥拉。同时西巴斯辛，这个之前从没有见过奥丽维娅的男子，由于被错认，直接就拉去结婚了。我只能说如果现实生活中的男女相爱有这个速度，我们国家的结婚率也不会这么低了。</t>
         </is>
       </c>
       <c r="H435" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/30785381/</t>
+          <t>https://book.douban.com/subject/30830398/</t>
         </is>
       </c>
     </row>
@@ -15808,12 +15808,12 @@
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>第十二夜</t>
+          <t>李尔王</t>
         </is>
       </c>
       <c r="C436" t="inlineStr">
         <is>
-          <t>朱生豪 / 译林出版社 / 35.90元</t>
+          <t>[英] 威廉·莎士比亚 / 朱生豪 / 译林出版社 / 39.80元</t>
         </is>
       </c>
       <c r="D436" s="2" t="n">
@@ -15829,12 +15829,12 @@
       </c>
       <c r="G436" t="inlineStr">
         <is>
-          <t>“别以为我这样向你求情，你就可以无须再献殷勤；须知求得的爱虽费心力，不劳而获的更应该珍惜。”威尼斯商人&amp;gt;无事生非&amp;gt;第十二夜&amp;gt;仲夏夜之梦。读的时候有好几次都有这样的感觉：为什么薇奥拉不直接表明自己的身份，亦或是听见有人错认自己的时候就直接拉着那个人问个清楚或去找自己的哥哥。如果这么干，这本书估计写到三分之一就结束了。结尾实在过于仓促了，当奥西诺被奥丽维娅拒绝且得知薇奥拉的真实身份之后，他居然立刻移情别恋，爱上了薇奥拉。同时西巴斯辛，这个之前从没有见过奥丽维娅的男子，由于被错认，直接就拉去结婚了。我只能说如果现实生活中的男女相爱有这个速度，我们国家的结婚率也不会这么低了。</t>
+          <t>如果说麦克白的悲剧是主人公的野心在预言和妻子的诱导下导致的咎由自取，奥赛罗的悲剧是主人公的冲动易怒的脾气和受小人蒙蔽的结果，那李尔王的悲剧就是李尔王作为一个父亲缺乏对女儿们的管教与了解导致的。“疯子带着瞎子走路，本来是这时代的一般病态。”，李尔王可以说既是疯子也是瞎子：他把自己所有的一切都交给了女儿们，而又没有交给真正最爱他的那个女儿。最后被两个利欲熏心的女儿敲骨吸髓，没能善终。李尔王的故事总让我想起电视里看到的那些晚景凄惨的老人：他们自己的孩子住在很好的房屋中，他们却只能在破旧的地方瑟瑟发抖。不过最让人伤心的还是格洛斯特：一个这么正直忠心的仆人，最后却落得了瞎眼身死的下场。</t>
         </is>
       </c>
       <c r="H436" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/30830398/</t>
+          <t>https://book.douban.com/subject/30785381/</t>
         </is>
       </c>
     </row>
@@ -16096,33 +16096,33 @@
       </c>
       <c r="B444" t="inlineStr">
         <is>
-          <t>死于威尼斯</t>
+          <t>红树林</t>
         </is>
       </c>
       <c r="C444" t="inlineStr">
         <is>
-          <t>[德] 托马斯·曼 / 钱鸿嘉、刘德中 / 上海译文出版社 / 2010-5 / 20.00元</t>
+          <t>莫言 / 浙江文艺出版社 / 2017-1 / 49.00元</t>
         </is>
       </c>
       <c r="D444" s="2" t="n">
         <v>45116</v>
       </c>
       <c r="E444" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F444" t="inlineStr">
         <is>
-          <t>外国文学 德语文学 #上海译文</t>
+          <t>汉语文学 现当代文学</t>
         </is>
       </c>
       <c r="G444" t="inlineStr">
         <is>
-          <t>“差不多所有伟大的事物都是“敢于藐视”的，是在跟忧虑、痛苦、穷困、孤独、病弱、道德败坏、七情六欲以及各种各样的障碍作斗争而诞生出来的。”“个性孤独、沉默寡言的人们，在观察和感受方面没有像合群的人们那样清晰敏锐，但比他们却更为深刻。前者的思路较为迟钝，但却神采飞扬，而且不无忧伤之情。在别人可以一顾了之、一笑置之或三言两语就可轻易作结论的景象和感受，却会盘踞在这种人的脑际，久久不能忘怀；它们默默地陷在里面，变得意味深长，同时也就成为经验、情感以及大胆的冒险精神。”“要是有谁观察过他，就一定会下一个结论：作家是这样一种人，写作对于他比对任何人都来得艰巨。”读了挺久也没读出好来，可能托马斯·曼不是我的菜吧……</t>
+          <t>“但淤泥塘也罢，变色蛇也罢，还不是最可怕的，这些东西毕竟还是可以避开的，只要你小心注意。红树林中最可怕的，是那些腐败的树叶子散出的腐气，很快就能让进入树林的人心醉神迷、精神恍惚，然后便迷迷糊糊地在树林里转圈，转呀转呀，怎么也转不出去，一直等到潮水汹涌地涨上来将人淹死。”同样是讲官场腐败，这本书读着就比《酒国》轻松。主要原因还是结构：《酒国》结果相比较而言更复杂，而这本书则更清楚。珍珠就是过去的林岚，单纯善良，相信别人，希望用自己的劳动堂堂正正地活着，也幻想着自己可以拥有简单朴素的爱情。可惜事与愿违，当林岚离开红树林的时候，她就注定踏入官场，美好的东西都随之消散。权，钱，色，名成为了她的枷锁，也成为了她控制别人的枷锁。这书尺度之大，描写之直接，放在现在可能是不能出版了。</t>
         </is>
       </c>
       <c r="H444" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/4621099/</t>
+          <t>https://book.douban.com/subject/26936013/</t>
         </is>
       </c>
     </row>
@@ -16132,33 +16132,33 @@
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>红树林</t>
+          <t>死于威尼斯</t>
         </is>
       </c>
       <c r="C445" t="inlineStr">
         <is>
-          <t>莫言 / 浙江文艺出版社 / 2017-1 / 49.00元</t>
+          <t>[德] 托马斯·曼 / 钱鸿嘉、刘德中 / 上海译文出版社 / 2010-5 / 20.00元</t>
         </is>
       </c>
       <c r="D445" s="2" t="n">
         <v>45116</v>
       </c>
       <c r="E445" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F445" t="inlineStr">
         <is>
-          <t>汉语文学 现当代文学</t>
+          <t>外国文学 德语文学 #上海译文</t>
         </is>
       </c>
       <c r="G445" t="inlineStr">
         <is>
-          <t>“但淤泥塘也罢，变色蛇也罢，还不是最可怕的，这些东西毕竟还是可以避开的，只要你小心注意。红树林中最可怕的，是那些腐败的树叶子散出的腐气，很快就能让进入树林的人心醉神迷、精神恍惚，然后便迷迷糊糊地在树林里转圈，转呀转呀，怎么也转不出去，一直等到潮水汹涌地涨上来将人淹死。”同样是讲官场腐败，这本书读着就比《酒国》轻松。主要原因还是结构：《酒国》结果相比较而言更复杂，而这本书则更清楚。珍珠就是过去的林岚，单纯善良，相信别人，希望用自己的劳动堂堂正正地活着，也幻想着自己可以拥有简单朴素的爱情。可惜事与愿违，当林岚离开红树林的时候，她就注定踏入官场，美好的东西都随之消散。权，钱，色，名成为了她的枷锁，也成为了她控制别人的枷锁。这书尺度之大，描写之直接，放在现在可能是不能出版了。</t>
+          <t>“差不多所有伟大的事物都是“敢于藐视”的，是在跟忧虑、痛苦、穷困、孤独、病弱、道德败坏、七情六欲以及各种各样的障碍作斗争而诞生出来的。”“个性孤独、沉默寡言的人们，在观察和感受方面没有像合群的人们那样清晰敏锐，但比他们却更为深刻。前者的思路较为迟钝，但却神采飞扬，而且不无忧伤之情。在别人可以一顾了之、一笑置之或三言两语就可轻易作结论的景象和感受，却会盘踞在这种人的脑际，久久不能忘怀；它们默默地陷在里面，变得意味深长，同时也就成为经验、情感以及大胆的冒险精神。”“要是有谁观察过他，就一定会下一个结论：作家是这样一种人，写作对于他比对任何人都来得艰巨。”读了挺久也没读出好来，可能托马斯·曼不是我的菜吧……</t>
         </is>
       </c>
       <c r="H445" t="inlineStr">
         <is>
-          <t>https://book.douban.com/subject/26936013/</t>
+          <t>https://book.douban.com/subject/4621099/</t>
         </is>
       </c>
     </row>
@@ -17779,6 +17779,42 @@
       <c r="H490" t="inlineStr">
         <is>
           <t>https://book.douban.com/subject/35096959/</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" s="1" t="n">
+        <v>489</v>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>爆炸</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>莫言 / 浙江文艺出版社 / 2020-7 / 46.00元</t>
+        </is>
+      </c>
+      <c r="D491" s="2" t="n">
+        <v>45773</v>
+      </c>
+      <c r="E491" t="n">
+        <v>4</v>
+      </c>
+      <c r="F491" t="inlineStr">
+        <is>
+          <t>汉语文学 现当代文学</t>
+        </is>
+      </c>
+      <c r="G491" t="inlineStr">
+        <is>
+          <t>《爆炸》描写了一个丈夫在得知妻子怀孕后，在特殊年代不得不带着妻子去流产。传统观念和现代思想，集体主义和个人想法，传宗接代和计划生育，这些纷纷碰撞在一起，形成一场大爆炸。已经有《蛙》的雏形。《欢乐》中一个农村贫困家庭中的有志青年想要通过高考跳出农村却屡战屡败，得了“高考综合征”。在最后一次失败后，他不堪其辱，终于喝下农药，结束痛苦，获得“欢乐”。《雨中的河》是军旅题材的小说，通过田夫的同事的回忆描写了一个虽然经历了生活苦痛，但是仍然选择贡献自己一生给国家的军人的故事。苦啊，苦啊，莫言笔下的人物总是被痛苦笼罩，被时代的洪流，社会的偏见，命运的捉弄所裹挟着前进。</t>
+        </is>
+      </c>
+      <c r="H491" t="inlineStr">
+        <is>
+          <t>https://book.douban.com/subject/35096965/</t>
         </is>
       </c>
     </row>

</xml_diff>